<commit_message>
Conf antichevirement sans pins
</commit_message>
<xml_diff>
--- a/Projet_voilier_conf.xlsx
+++ b/Projet_voilier_conf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/428acea97df47522/Images/Documents/GitHub/Voilier/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Downloads\fime joseph\9no\Microcontrolleurs\Voilier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44E492FB-4378-461D-80CC-598B9B5E3F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6824DCB4-FFD9-463A-9C95-F9D42EC9C141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E824238D-CECB-4533-AA98-D1D470E3A7AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E824238D-CECB-4533-AA98-D1D470E3A7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Fonction </t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Plateau.c</t>
+  </si>
+  <si>
+    <t>Anti-chavirement</t>
+  </si>
+  <si>
+    <t>Accelerometre.c</t>
+  </si>
+  <si>
+    <t>SPI1</t>
   </si>
 </sst>
 </file>
@@ -294,172 +303,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -471,29 +327,197 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +538,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -812,334 +836,347 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2620248D-B346-418B-BDB4-C0777BAFED66}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="24.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="61"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="62"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="63"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="64"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E11" s="2" t="s">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E11" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="62"/>
+      <c r="G11" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="2" t="s">
+      <c r="H11" s="62"/>
+      <c r="I11" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="2" t="s">
+      <c r="J11" s="62"/>
+      <c r="K11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="2" t="s">
+      <c r="L11" s="65"/>
+      <c r="M11" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="18"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="11"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="5:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E17" s="74" t="s">
+      <c r="N11" s="62"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="5:14" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="74" t="s">
+      <c r="F17" s="68"/>
+      <c r="G17" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="62" t="s">
+      <c r="H17" s="33"/>
+      <c r="I17" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="67"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="11"/>
-    </row>
-    <row r="18" spans="5:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="62" t="s">
+      <c r="J17" s="26"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="5:14" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="68"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="11"/>
-    </row>
-    <row r="19" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="60" t="s">
+      <c r="J18" s="27"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="69"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="70"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="13"/>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="11"/>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="11"/>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="11"/>
-    </row>
-    <row r="25" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="75" t="s">
+      <c r="J19" s="29"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="77"/>
+      <c r="G21" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="77"/>
+      <c r="I21" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="78"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="78"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="78"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="80"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="76" t="s">
+      <c r="F26" s="39"/>
+      <c r="G26" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="45"/>
-      <c r="I26" s="44" t="s">
+      <c r="H26" s="20"/>
+      <c r="I26" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="45"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="51" t="s">
         <v>9</v>
       </c>
       <c r="L26" s="52"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="24"/>
-    </row>
-    <row r="27" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="47"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="45"/>
+    </row>
+    <row r="27" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="53"/>
       <c r="L27" s="54"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="27"/>
-    </row>
-    <row r="28" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="50" t="s">
+      <c r="M27" s="46"/>
+      <c r="N27" s="47"/>
+    </row>
+    <row r="28" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="L28" s="55"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="24"/>
-    </row>
-    <row r="29" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="25"/>
-    </row>
-    <row r="30" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="27"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="45"/>
+    </row>
+    <row r="29" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="49"/>
+    </row>
+    <row r="30" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="G26:H30"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J20"/>
-    <mergeCell ref="G17:H20"/>
+  <mergeCells count="25">
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="E21:F25"/>
+    <mergeCell ref="G21:H25"/>
+    <mergeCell ref="I21:J25"/>
+    <mergeCell ref="E17:F20"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="M11:N12"/>
     <mergeCell ref="E26:F30"/>
     <mergeCell ref="M26:N27"/>
     <mergeCell ref="M28:N30"/>
     <mergeCell ref="I26:J30"/>
     <mergeCell ref="K26:L27"/>
     <mergeCell ref="K28:L30"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="E17:F20"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="E1:F2"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="G26:H30"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J20"/>
+    <mergeCell ref="G17:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pins utilisés par SPI dans l'excel
</commit_message>
<xml_diff>
--- a/Projet_voilier_conf.xlsx
+++ b/Projet_voilier_conf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/428acea97df47522/Images/Documents/GitHub/Voilier/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Downloads\fime joseph\9no\Microcontrolleurs\Voilier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{44E492FB-4378-461D-80CC-598B9B5E3F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1ABD1C3-7032-48CB-B195-1C77A0B8E9F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802044F9-2A3F-43B2-9338-6B1A27D2EAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E824238D-CECB-4533-AA98-D1D470E3A7AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E824238D-CECB-4533-AA98-D1D470E3A7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">Fonction </t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>en Input Pull-up</t>
+  </si>
+  <si>
+    <t>Projet Anti-chevirement</t>
+  </si>
+  <si>
+    <t>Antichevirement.c</t>
+  </si>
+  <si>
+    <t>SPI,GPIO</t>
+  </si>
+  <si>
+    <t>SPI1_SCK : PA.5</t>
+  </si>
+  <si>
+    <t>SPI1_NSS : PA.4</t>
+  </si>
+  <si>
+    <t>SPI1_MISO : PA.6</t>
+  </si>
+  <si>
+    <t>SPI_MOSI : PA.7</t>
+  </si>
+  <si>
+    <t>Alternate function output Push-pull</t>
+  </si>
+  <si>
+    <t>Floating input</t>
+  </si>
+  <si>
+    <t>General Open-drain output</t>
   </si>
 </sst>
 </file>
@@ -308,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -317,7 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -336,22 +365,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -375,9 +509,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,125 +524,58 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +595,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -829,75 +893,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2620248D-B346-418B-BDB4-C0777BAFED66}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="48.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.21875" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="23.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="60"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="61"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="62"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="63"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E11" s="60" t="s">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E11" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="60" t="s">
+      <c r="F11" s="19"/>
+      <c r="G11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="60" t="s">
+      <c r="H11" s="19"/>
+      <c r="I11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="60" t="s">
+      <c r="J11" s="19"/>
+      <c r="K11" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="64"/>
-      <c r="M11" s="60" t="s">
+      <c r="L11" s="32"/>
+      <c r="M11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="61"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E12" s="62"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="63"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="30"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="6"/>
@@ -909,7 +979,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2"/>
@@ -921,7 +991,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2"/>
@@ -933,7 +1003,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="G16" s="4"/>
@@ -945,209 +1015,232 @@
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="5:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E17" s="32" t="s">
+    <row r="17" spans="5:14" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="32" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="25" t="s">
+      <c r="H17" s="66"/>
+      <c r="I17" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="9"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="8"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="5:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="25" t="s">
+    <row r="18" spans="5:14" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="9"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="8"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="28" t="s">
+    <row r="19" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="9"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="8"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="70"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="10"/>
+    <row r="20" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="10"/>
+    <row r="21" spans="5:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="71"/>
+      <c r="G21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="71"/>
+      <c r="I21" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="43"/>
+      <c r="K21" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="78"/>
+      <c r="M21" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="N21" s="36"/>
+    </row>
+    <row r="22" spans="5:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E22" s="72"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="78"/>
+      <c r="M22" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="41"/>
+    </row>
+    <row r="23" spans="5:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E23" s="72"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="78"/>
+      <c r="M23" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" s="41"/>
+    </row>
+    <row r="24" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E24" s="72"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="78"/>
+      <c r="M24" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="41"/>
+    </row>
+    <row r="25" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E25" s="74"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="38" t="s">
+    <row r="26" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="19" t="s">
+      <c r="F26" s="85"/>
+      <c r="G26" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="49" t="s">
+      <c r="H26" s="43"/>
+      <c r="I26" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="50" t="s">
+      <c r="J26" s="43"/>
+      <c r="K26" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="77" t="s">
+      <c r="L26" s="49"/>
+      <c r="M26" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N26" s="44"/>
-    </row>
-    <row r="27" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E27" s="40"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="46"/>
-    </row>
-    <row r="28" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="54" t="s">
+      <c r="N26" s="81"/>
+    </row>
+    <row r="27" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="86"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="83"/>
+    </row>
+    <row r="28" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L28" s="55"/>
-      <c r="M28" s="76" t="s">
+      <c r="L28" s="53"/>
+      <c r="M28" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="N28" s="44"/>
-    </row>
-    <row r="29" spans="5:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="48"/>
-    </row>
-    <row r="30" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="46"/>
+      <c r="N28" s="36"/>
+    </row>
+    <row r="29" spans="5:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="41"/>
+    </row>
+    <row r="30" spans="5:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="88"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="I1:J2"/>
-    <mergeCell ref="E17:F20"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="E1:F2"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
+  <mergeCells count="33">
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="G21:H25"/>
+    <mergeCell ref="I21:J25"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
     <mergeCell ref="K11:L12"/>
     <mergeCell ref="M11:N12"/>
     <mergeCell ref="E26:F30"/>
@@ -1161,6 +1254,16 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="I19:J20"/>
     <mergeCell ref="G17:H20"/>
+    <mergeCell ref="E21:F25"/>
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="E17:F20"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>